<commit_message>
Atualiza dados da liga classica
</commit_message>
<xml_diff>
--- a/liga_classica/datasets_liga_classica/Pontuacoes_Liga_Classica_Completa.xlsx
+++ b/liga_classica/datasets_liga_classica/Pontuacoes_Liga_Classica_Completa.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="90">
   <si>
     <t>Rodada 1</t>
   </si>
@@ -274,6 +274,9 @@
   </si>
   <si>
     <t>Tatols Beants F.C</t>
+  </si>
+  <si>
+    <t>TEAM LOPES 99</t>
   </si>
   <si>
     <t>teves_futsal20 f.c</t>
@@ -646,7 +649,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AM52"/>
+  <dimension ref="A1:AM53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -6837,6 +6840,125 @@
         <v>0</v>
       </c>
     </row>
+    <row r="53" spans="1:39">
+      <c r="A53" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B53">
+        <v>0</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+      <c r="F53">
+        <v>0</v>
+      </c>
+      <c r="G53">
+        <v>0</v>
+      </c>
+      <c r="H53">
+        <v>0</v>
+      </c>
+      <c r="I53">
+        <v>0</v>
+      </c>
+      <c r="J53">
+        <v>0</v>
+      </c>
+      <c r="K53">
+        <v>0</v>
+      </c>
+      <c r="L53">
+        <v>0</v>
+      </c>
+      <c r="M53">
+        <v>0</v>
+      </c>
+      <c r="N53">
+        <v>0</v>
+      </c>
+      <c r="O53">
+        <v>0</v>
+      </c>
+      <c r="P53">
+        <v>0</v>
+      </c>
+      <c r="Q53">
+        <v>0</v>
+      </c>
+      <c r="R53">
+        <v>0</v>
+      </c>
+      <c r="S53">
+        <v>0</v>
+      </c>
+      <c r="T53">
+        <v>0</v>
+      </c>
+      <c r="U53">
+        <v>0</v>
+      </c>
+      <c r="V53">
+        <v>0</v>
+      </c>
+      <c r="W53">
+        <v>0</v>
+      </c>
+      <c r="X53">
+        <v>0</v>
+      </c>
+      <c r="Y53">
+        <v>0</v>
+      </c>
+      <c r="Z53">
+        <v>0</v>
+      </c>
+      <c r="AA53">
+        <v>0</v>
+      </c>
+      <c r="AB53">
+        <v>0</v>
+      </c>
+      <c r="AC53">
+        <v>0</v>
+      </c>
+      <c r="AD53">
+        <v>0</v>
+      </c>
+      <c r="AE53">
+        <v>0</v>
+      </c>
+      <c r="AF53">
+        <v>0</v>
+      </c>
+      <c r="AG53">
+        <v>0</v>
+      </c>
+      <c r="AH53">
+        <v>0</v>
+      </c>
+      <c r="AI53">
+        <v>0</v>
+      </c>
+      <c r="AJ53">
+        <v>0</v>
+      </c>
+      <c r="AK53">
+        <v>0</v>
+      </c>
+      <c r="AL53">
+        <v>0</v>
+      </c>
+      <c r="AM53">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6844,7 +6966,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T52"/>
+  <dimension ref="A1:T53"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -10071,6 +10193,68 @@
         <v>0</v>
       </c>
     </row>
+    <row r="53" spans="1:20">
+      <c r="A53" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B53">
+        <v>0</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+      <c r="F53">
+        <v>0</v>
+      </c>
+      <c r="G53">
+        <v>0</v>
+      </c>
+      <c r="H53">
+        <v>0</v>
+      </c>
+      <c r="I53">
+        <v>0</v>
+      </c>
+      <c r="J53">
+        <v>0</v>
+      </c>
+      <c r="K53">
+        <v>0</v>
+      </c>
+      <c r="L53">
+        <v>0</v>
+      </c>
+      <c r="M53">
+        <v>0</v>
+      </c>
+      <c r="N53">
+        <v>0</v>
+      </c>
+      <c r="O53">
+        <v>0</v>
+      </c>
+      <c r="P53">
+        <v>0</v>
+      </c>
+      <c r="Q53">
+        <v>0</v>
+      </c>
+      <c r="R53">
+        <v>0</v>
+      </c>
+      <c r="S53">
+        <v>0</v>
+      </c>
+      <c r="T53">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10078,7 +10262,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B52"/>
+  <dimension ref="A1:B53"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -10099,7 +10283,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>76</v>
+        <v>39</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -10187,7 +10371,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -10195,7 +10379,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -10283,7 +10467,7 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="1" t="s">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -10291,7 +10475,7 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -10299,7 +10483,7 @@
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="1" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -10307,7 +10491,7 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="1" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -10315,7 +10499,7 @@
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="1" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B30">
         <v>0</v>
@@ -10323,7 +10507,7 @@
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B31">
         <v>0</v>
@@ -10331,7 +10515,7 @@
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B32">
         <v>0</v>
@@ -10339,7 +10523,7 @@
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B33">
         <v>0</v>
@@ -10347,7 +10531,7 @@
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -10355,7 +10539,7 @@
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B35">
         <v>0</v>
@@ -10363,7 +10547,7 @@
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B36">
         <v>0</v>
@@ -10371,7 +10555,7 @@
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B37">
         <v>0</v>
@@ -10379,7 +10563,7 @@
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -10387,7 +10571,7 @@
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -10395,7 +10579,7 @@
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -10403,7 +10587,7 @@
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="1" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -10411,7 +10595,7 @@
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="1" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -10419,7 +10603,7 @@
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B43">
         <v>0</v>
@@ -10427,7 +10611,7 @@
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B44">
         <v>0</v>
@@ -10435,7 +10619,7 @@
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -10443,7 +10627,7 @@
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B46">
         <v>0</v>
@@ -10451,7 +10635,7 @@
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B47">
         <v>0</v>
@@ -10459,7 +10643,7 @@
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B48">
         <v>0</v>
@@ -10467,7 +10651,7 @@
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B49">
         <v>0</v>
@@ -10475,7 +10659,7 @@
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B50">
         <v>0</v>
@@ -10483,7 +10667,7 @@
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B51">
         <v>0</v>
@@ -10491,9 +10675,17 @@
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="1" t="s">
-        <v>88</v>
+        <v>61</v>
       </c>
       <c r="B52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B53">
         <v>0</v>
       </c>
     </row>
@@ -10504,7 +10696,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B52"/>
+  <dimension ref="A1:B53"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -10525,7 +10717,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>76</v>
+        <v>39</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -10613,7 +10805,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -10621,7 +10813,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -10709,7 +10901,7 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="1" t="s">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -10717,7 +10909,7 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -10725,7 +10917,7 @@
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="1" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -10733,7 +10925,7 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="1" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -10741,7 +10933,7 @@
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="1" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B30">
         <v>0</v>
@@ -10749,7 +10941,7 @@
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B31">
         <v>0</v>
@@ -10757,7 +10949,7 @@
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B32">
         <v>0</v>
@@ -10765,7 +10957,7 @@
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B33">
         <v>0</v>
@@ -10773,7 +10965,7 @@
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -10781,7 +10973,7 @@
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B35">
         <v>0</v>
@@ -10789,7 +10981,7 @@
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B36">
         <v>0</v>
@@ -10797,7 +10989,7 @@
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B37">
         <v>0</v>
@@ -10805,7 +10997,7 @@
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -10813,7 +11005,7 @@
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -10821,7 +11013,7 @@
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -10829,7 +11021,7 @@
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="1" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -10837,7 +11029,7 @@
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="1" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -10845,7 +11037,7 @@
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B43">
         <v>0</v>
@@ -10853,7 +11045,7 @@
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B44">
         <v>0</v>
@@ -10861,7 +11053,7 @@
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -10869,7 +11061,7 @@
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B46">
         <v>0</v>
@@ -10877,7 +11069,7 @@
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B47">
         <v>0</v>
@@ -10885,7 +11077,7 @@
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B48">
         <v>0</v>
@@ -10893,7 +11085,7 @@
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B49">
         <v>0</v>
@@ -10901,7 +11093,7 @@
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B50">
         <v>0</v>
@@ -10909,7 +11101,7 @@
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B51">
         <v>0</v>
@@ -10917,9 +11109,17 @@
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="1" t="s">
-        <v>88</v>
+        <v>61</v>
       </c>
       <c r="B52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B53">
         <v>0</v>
       </c>
     </row>
@@ -10930,7 +11130,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B52"/>
+  <dimension ref="A1:B53"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -10951,7 +11151,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>76</v>
+        <v>39</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -11039,7 +11239,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -11047,7 +11247,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -11135,7 +11335,7 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="1" t="s">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -11143,7 +11343,7 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -11151,7 +11351,7 @@
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="1" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -11159,7 +11359,7 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="1" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -11167,7 +11367,7 @@
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="1" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B30">
         <v>0</v>
@@ -11175,7 +11375,7 @@
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B31">
         <v>0</v>
@@ -11183,7 +11383,7 @@
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B32">
         <v>0</v>
@@ -11191,7 +11391,7 @@
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B33">
         <v>0</v>
@@ -11199,7 +11399,7 @@
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -11207,7 +11407,7 @@
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B35">
         <v>0</v>
@@ -11215,7 +11415,7 @@
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B36">
         <v>0</v>
@@ -11223,7 +11423,7 @@
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B37">
         <v>0</v>
@@ -11231,7 +11431,7 @@
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -11239,7 +11439,7 @@
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -11247,7 +11447,7 @@
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -11255,7 +11455,7 @@
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="1" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -11263,7 +11463,7 @@
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="1" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -11271,7 +11471,7 @@
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B43">
         <v>0</v>
@@ -11279,7 +11479,7 @@
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B44">
         <v>0</v>
@@ -11287,7 +11487,7 @@
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -11295,7 +11495,7 @@
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B46">
         <v>0</v>
@@ -11303,7 +11503,7 @@
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B47">
         <v>0</v>
@@ -11311,7 +11511,7 @@
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B48">
         <v>0</v>
@@ -11319,7 +11519,7 @@
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B49">
         <v>0</v>
@@ -11327,7 +11527,7 @@
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B50">
         <v>0</v>
@@ -11335,7 +11535,7 @@
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B51">
         <v>0</v>
@@ -11343,9 +11543,17 @@
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="1" t="s">
-        <v>88</v>
+        <v>61</v>
       </c>
       <c r="B52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B53">
         <v>0</v>
       </c>
     </row>
@@ -11356,7 +11564,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B52"/>
+  <dimension ref="A1:B53"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -11377,7 +11585,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>76</v>
+        <v>39</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -11465,7 +11673,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -11473,7 +11681,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -11561,7 +11769,7 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="1" t="s">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -11569,7 +11777,7 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -11577,7 +11785,7 @@
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="1" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -11585,7 +11793,7 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="1" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -11593,7 +11801,7 @@
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="1" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B30">
         <v>0</v>
@@ -11601,7 +11809,7 @@
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B31">
         <v>0</v>
@@ -11609,7 +11817,7 @@
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B32">
         <v>0</v>
@@ -11617,7 +11825,7 @@
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B33">
         <v>0</v>
@@ -11625,7 +11833,7 @@
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -11633,7 +11841,7 @@
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B35">
         <v>0</v>
@@ -11641,7 +11849,7 @@
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B36">
         <v>0</v>
@@ -11649,7 +11857,7 @@
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B37">
         <v>0</v>
@@ -11657,7 +11865,7 @@
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -11665,7 +11873,7 @@
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -11673,7 +11881,7 @@
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -11681,7 +11889,7 @@
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="1" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -11689,7 +11897,7 @@
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="1" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -11697,7 +11905,7 @@
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B43">
         <v>0</v>
@@ -11705,7 +11913,7 @@
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B44">
         <v>0</v>
@@ -11713,7 +11921,7 @@
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -11721,7 +11929,7 @@
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B46">
         <v>0</v>
@@ -11729,7 +11937,7 @@
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B47">
         <v>0</v>
@@ -11737,7 +11945,7 @@
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B48">
         <v>0</v>
@@ -11745,7 +11953,7 @@
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B49">
         <v>0</v>
@@ -11753,7 +11961,7 @@
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B50">
         <v>0</v>
@@ -11761,7 +11969,7 @@
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B51">
         <v>0</v>
@@ -11769,9 +11977,17 @@
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="1" t="s">
-        <v>88</v>
+        <v>61</v>
       </c>
       <c r="B52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B53">
         <v>0</v>
       </c>
     </row>
@@ -11782,7 +11998,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B52"/>
+  <dimension ref="A1:B53"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -11803,7 +12019,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>76</v>
+        <v>39</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -11891,7 +12107,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -11899,7 +12115,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -11987,7 +12203,7 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="1" t="s">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -11995,7 +12211,7 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -12003,7 +12219,7 @@
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="1" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -12011,7 +12227,7 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="1" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -12019,7 +12235,7 @@
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="1" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B30">
         <v>0</v>
@@ -12027,7 +12243,7 @@
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B31">
         <v>0</v>
@@ -12035,7 +12251,7 @@
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B32">
         <v>0</v>
@@ -12043,7 +12259,7 @@
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B33">
         <v>0</v>
@@ -12051,7 +12267,7 @@
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -12059,7 +12275,7 @@
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B35">
         <v>0</v>
@@ -12067,7 +12283,7 @@
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B36">
         <v>0</v>
@@ -12075,7 +12291,7 @@
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B37">
         <v>0</v>
@@ -12083,7 +12299,7 @@
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -12091,7 +12307,7 @@
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -12099,7 +12315,7 @@
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -12107,7 +12323,7 @@
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="1" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -12115,7 +12331,7 @@
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="1" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -12123,7 +12339,7 @@
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B43">
         <v>0</v>
@@ -12131,7 +12347,7 @@
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B44">
         <v>0</v>
@@ -12139,7 +12355,7 @@
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -12147,7 +12363,7 @@
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B46">
         <v>0</v>
@@ -12155,7 +12371,7 @@
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B47">
         <v>0</v>
@@ -12163,7 +12379,7 @@
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B48">
         <v>0</v>
@@ -12171,7 +12387,7 @@
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B49">
         <v>0</v>
@@ -12179,7 +12395,7 @@
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B50">
         <v>0</v>
@@ -12187,7 +12403,7 @@
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B51">
         <v>0</v>
@@ -12195,9 +12411,17 @@
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="1" t="s">
-        <v>88</v>
+        <v>61</v>
       </c>
       <c r="B52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B53">
         <v>0</v>
       </c>
     </row>
@@ -12208,7 +12432,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B52"/>
+  <dimension ref="A1:B53"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -12229,7 +12453,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>76</v>
+        <v>39</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -12317,7 +12541,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -12325,7 +12549,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -12413,7 +12637,7 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="1" t="s">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -12421,7 +12645,7 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -12429,7 +12653,7 @@
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="1" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -12437,7 +12661,7 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="1" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -12445,7 +12669,7 @@
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="1" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B30">
         <v>0</v>
@@ -12453,7 +12677,7 @@
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B31">
         <v>0</v>
@@ -12461,7 +12685,7 @@
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B32">
         <v>0</v>
@@ -12469,7 +12693,7 @@
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B33">
         <v>0</v>
@@ -12477,7 +12701,7 @@
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -12485,7 +12709,7 @@
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B35">
         <v>0</v>
@@ -12493,7 +12717,7 @@
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B36">
         <v>0</v>
@@ -12501,7 +12725,7 @@
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B37">
         <v>0</v>
@@ -12509,7 +12733,7 @@
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -12517,7 +12741,7 @@
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -12525,7 +12749,7 @@
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -12533,7 +12757,7 @@
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="1" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -12541,7 +12765,7 @@
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="1" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -12549,7 +12773,7 @@
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B43">
         <v>0</v>
@@ -12557,7 +12781,7 @@
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B44">
         <v>0</v>
@@ -12565,7 +12789,7 @@
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -12573,7 +12797,7 @@
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B46">
         <v>0</v>
@@ -12581,7 +12805,7 @@
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B47">
         <v>0</v>
@@ -12589,7 +12813,7 @@
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B48">
         <v>0</v>
@@ -12597,7 +12821,7 @@
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B49">
         <v>0</v>
@@ -12605,7 +12829,7 @@
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B50">
         <v>0</v>
@@ -12613,7 +12837,7 @@
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B51">
         <v>0</v>
@@ -12621,9 +12845,17 @@
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="1" t="s">
-        <v>88</v>
+        <v>61</v>
       </c>
       <c r="B52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B53">
         <v>0</v>
       </c>
     </row>
@@ -12634,7 +12866,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B52"/>
+  <dimension ref="A1:B53"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -12655,7 +12887,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>76</v>
+        <v>39</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -12743,7 +12975,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -12751,7 +12983,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -12839,7 +13071,7 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="1" t="s">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -12847,7 +13079,7 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -12855,7 +13087,7 @@
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="1" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -12863,7 +13095,7 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="1" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -12871,7 +13103,7 @@
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="1" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B30">
         <v>0</v>
@@ -12879,7 +13111,7 @@
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B31">
         <v>0</v>
@@ -12887,7 +13119,7 @@
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B32">
         <v>0</v>
@@ -12895,7 +13127,7 @@
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B33">
         <v>0</v>
@@ -12903,7 +13135,7 @@
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -12911,7 +13143,7 @@
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B35">
         <v>0</v>
@@ -12919,7 +13151,7 @@
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B36">
         <v>0</v>
@@ -12927,7 +13159,7 @@
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B37">
         <v>0</v>
@@ -12935,7 +13167,7 @@
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -12943,7 +13175,7 @@
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -12951,7 +13183,7 @@
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -12959,7 +13191,7 @@
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="1" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -12967,7 +13199,7 @@
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="1" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -12975,7 +13207,7 @@
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B43">
         <v>0</v>
@@ -12983,7 +13215,7 @@
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B44">
         <v>0</v>
@@ -12991,7 +13223,7 @@
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -12999,7 +13231,7 @@
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B46">
         <v>0</v>
@@ -13007,7 +13239,7 @@
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B47">
         <v>0</v>
@@ -13015,7 +13247,7 @@
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B48">
         <v>0</v>
@@ -13023,7 +13255,7 @@
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B49">
         <v>0</v>
@@ -13031,7 +13263,7 @@
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B50">
         <v>0</v>
@@ -13039,7 +13271,7 @@
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B51">
         <v>0</v>
@@ -13047,9 +13279,17 @@
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="1" t="s">
-        <v>88</v>
+        <v>61</v>
       </c>
       <c r="B52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B53">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualiza parciais na Liga Classica
</commit_message>
<xml_diff>
--- a/liga_classica/datasets_liga_classica/Pontuacoes_Liga_Classica_Completa.xlsx
+++ b/liga_classica/datasets_liga_classica/Pontuacoes_Liga_Classica_Completa.xlsx
@@ -10,19 +10,19 @@
     <sheet name="Geral" sheetId="1" r:id="rId1"/>
     <sheet name="Turno 2" sheetId="2" r:id="rId2"/>
     <sheet name="Classif Turno 2" sheetId="3" r:id="rId3"/>
-    <sheet name="Mês - Janeiro" sheetId="4" r:id="rId4"/>
-    <sheet name="Mês - Fevereiro" sheetId="5" r:id="rId5"/>
-    <sheet name="Mês - Março" sheetId="6" r:id="rId6"/>
-    <sheet name="Mês - Abril" sheetId="7" r:id="rId7"/>
-    <sheet name="Mês - Maio" sheetId="8" r:id="rId8"/>
-    <sheet name="Mês - Julho" sheetId="9" r:id="rId9"/>
+    <sheet name="Mes - Janeiro" sheetId="4" r:id="rId4"/>
+    <sheet name="Mes - Fevereiro" sheetId="5" r:id="rId5"/>
+    <sheet name="Mes - Marco" sheetId="6" r:id="rId6"/>
+    <sheet name="Mes - Abril" sheetId="7" r:id="rId7"/>
+    <sheet name="Mes - Maio" sheetId="8" r:id="rId8"/>
+    <sheet name="Mes - Julho" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="91">
   <si>
     <t>Rodada 1</t>
   </si>
@@ -292,6 +292,9 @@
   </si>
   <si>
     <t>VASCO MARTINS FC</t>
+  </si>
+  <si>
+    <t>Lider_Rodada</t>
   </si>
 </sst>
 </file>
@@ -649,7 +652,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AM53"/>
+  <dimension ref="A1:AM54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -776,7 +779,7 @@
         <v>38</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>59.56</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -895,7 +898,7 @@
         <v>39</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>45.3</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -1014,7 +1017,7 @@
         <v>40</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>30.06</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -1133,7 +1136,7 @@
         <v>41</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>69.56</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -1252,7 +1255,7 @@
         <v>42</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>54.06</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -1371,7 +1374,7 @@
         <v>43</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>71.70999999999999</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -1490,7 +1493,7 @@
         <v>44</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>53.06</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -1609,7 +1612,7 @@
         <v>45</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>69.26000000000001</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -1728,7 +1731,7 @@
         <v>46</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>71.36</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -1847,7 +1850,7 @@
         <v>47</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>47.2</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -1966,7 +1969,7 @@
         <v>48</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>58.4</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -2085,7 +2088,7 @@
         <v>49</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>45.46</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -2204,7 +2207,7 @@
         <v>50</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>48.46</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -2323,7 +2326,7 @@
         <v>51</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>30.32</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -2442,7 +2445,7 @@
         <v>52</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>52.36</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -2561,7 +2564,7 @@
         <v>53</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>50.6</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -2680,7 +2683,7 @@
         <v>54</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>44.06</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -2799,7 +2802,7 @@
         <v>55</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>49.16</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -2918,7 +2921,7 @@
         <v>56</v>
       </c>
       <c r="B20">
-        <v>0</v>
+        <v>21.7</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -3037,7 +3040,7 @@
         <v>57</v>
       </c>
       <c r="B21">
-        <v>0</v>
+        <v>56.65</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -3156,7 +3159,7 @@
         <v>58</v>
       </c>
       <c r="B22">
-        <v>0</v>
+        <v>43.1</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -3275,7 +3278,7 @@
         <v>59</v>
       </c>
       <c r="B23">
-        <v>0</v>
+        <v>41.6</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -3394,7 +3397,7 @@
         <v>60</v>
       </c>
       <c r="B24">
-        <v>0</v>
+        <v>39.66</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -3513,7 +3516,7 @@
         <v>61</v>
       </c>
       <c r="B25">
-        <v>0</v>
+        <v>39.66</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -3632,7 +3635,7 @@
         <v>62</v>
       </c>
       <c r="B26">
-        <v>0</v>
+        <v>54.36</v>
       </c>
       <c r="C26">
         <v>0</v>
@@ -3751,7 +3754,7 @@
         <v>63</v>
       </c>
       <c r="B27">
-        <v>0</v>
+        <v>58.26</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -3870,7 +3873,7 @@
         <v>64</v>
       </c>
       <c r="B28">
-        <v>0</v>
+        <v>58.51</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -3989,7 +3992,7 @@
         <v>65</v>
       </c>
       <c r="B29">
-        <v>0</v>
+        <v>69.76000000000001</v>
       </c>
       <c r="C29">
         <v>0</v>
@@ -4108,7 +4111,7 @@
         <v>66</v>
       </c>
       <c r="B30">
-        <v>0</v>
+        <v>47.66</v>
       </c>
       <c r="C30">
         <v>0</v>
@@ -4227,7 +4230,7 @@
         <v>67</v>
       </c>
       <c r="B31">
-        <v>0</v>
+        <v>45.86</v>
       </c>
       <c r="C31">
         <v>0</v>
@@ -4346,7 +4349,7 @@
         <v>68</v>
       </c>
       <c r="B32">
-        <v>0</v>
+        <v>23.26</v>
       </c>
       <c r="C32">
         <v>0</v>
@@ -4465,7 +4468,7 @@
         <v>69</v>
       </c>
       <c r="B33">
-        <v>0</v>
+        <v>73.66</v>
       </c>
       <c r="C33">
         <v>0</v>
@@ -4584,7 +4587,7 @@
         <v>70</v>
       </c>
       <c r="B34">
-        <v>0</v>
+        <v>60.36</v>
       </c>
       <c r="C34">
         <v>0</v>
@@ -4703,7 +4706,7 @@
         <v>71</v>
       </c>
       <c r="B35">
-        <v>0</v>
+        <v>26.51</v>
       </c>
       <c r="C35">
         <v>0</v>
@@ -4822,7 +4825,7 @@
         <v>72</v>
       </c>
       <c r="B36">
-        <v>0</v>
+        <v>48.06</v>
       </c>
       <c r="C36">
         <v>0</v>
@@ -4941,7 +4944,7 @@
         <v>73</v>
       </c>
       <c r="B37">
-        <v>0</v>
+        <v>60.66</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -5060,7 +5063,7 @@
         <v>74</v>
       </c>
       <c r="B38">
-        <v>0</v>
+        <v>51.05</v>
       </c>
       <c r="C38">
         <v>0</v>
@@ -5179,7 +5182,7 @@
         <v>75</v>
       </c>
       <c r="B39">
-        <v>0</v>
+        <v>59.76</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -5298,7 +5301,7 @@
         <v>76</v>
       </c>
       <c r="B40">
-        <v>0</v>
+        <v>34.36</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -5417,7 +5420,7 @@
         <v>77</v>
       </c>
       <c r="B41">
-        <v>0</v>
+        <v>38.5</v>
       </c>
       <c r="C41">
         <v>0</v>
@@ -5536,7 +5539,7 @@
         <v>78</v>
       </c>
       <c r="B42">
-        <v>0</v>
+        <v>55.96</v>
       </c>
       <c r="C42">
         <v>0</v>
@@ -5655,7 +5658,7 @@
         <v>79</v>
       </c>
       <c r="B43">
-        <v>0</v>
+        <v>34.76</v>
       </c>
       <c r="C43">
         <v>0</v>
@@ -5774,7 +5777,7 @@
         <v>80</v>
       </c>
       <c r="B44">
-        <v>0</v>
+        <v>45.3</v>
       </c>
       <c r="C44">
         <v>0</v>
@@ -5893,7 +5896,7 @@
         <v>81</v>
       </c>
       <c r="B45">
-        <v>0</v>
+        <v>57.76</v>
       </c>
       <c r="C45">
         <v>0</v>
@@ -6012,7 +6015,7 @@
         <v>82</v>
       </c>
       <c r="B46">
-        <v>0</v>
+        <v>50.1</v>
       </c>
       <c r="C46">
         <v>0</v>
@@ -6131,7 +6134,7 @@
         <v>83</v>
       </c>
       <c r="B47">
-        <v>0</v>
+        <v>64.95999999999999</v>
       </c>
       <c r="C47">
         <v>0</v>
@@ -6250,7 +6253,7 @@
         <v>84</v>
       </c>
       <c r="B48">
-        <v>0</v>
+        <v>50.76</v>
       </c>
       <c r="C48">
         <v>0</v>
@@ -6369,7 +6372,7 @@
         <v>85</v>
       </c>
       <c r="B49">
-        <v>0</v>
+        <v>61.8</v>
       </c>
       <c r="C49">
         <v>0</v>
@@ -6488,7 +6491,7 @@
         <v>86</v>
       </c>
       <c r="B50">
-        <v>0</v>
+        <v>59.86</v>
       </c>
       <c r="C50">
         <v>0</v>
@@ -6607,7 +6610,7 @@
         <v>87</v>
       </c>
       <c r="B51">
-        <v>0</v>
+        <v>46.56</v>
       </c>
       <c r="C51">
         <v>0</v>
@@ -6726,7 +6729,7 @@
         <v>88</v>
       </c>
       <c r="B52">
-        <v>0</v>
+        <v>63.66</v>
       </c>
       <c r="C52">
         <v>0</v>
@@ -6845,7 +6848,7 @@
         <v>89</v>
       </c>
       <c r="B53">
-        <v>0</v>
+        <v>35.8</v>
       </c>
       <c r="C53">
         <v>0</v>
@@ -6956,6 +6959,125 @@
         <v>0</v>
       </c>
       <c r="AM53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:39">
+      <c r="A54" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B54">
+        <v>0</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="E54">
+        <v>0</v>
+      </c>
+      <c r="F54">
+        <v>0</v>
+      </c>
+      <c r="G54">
+        <v>0</v>
+      </c>
+      <c r="H54">
+        <v>0</v>
+      </c>
+      <c r="I54">
+        <v>0</v>
+      </c>
+      <c r="J54">
+        <v>0</v>
+      </c>
+      <c r="K54">
+        <v>0</v>
+      </c>
+      <c r="L54">
+        <v>0</v>
+      </c>
+      <c r="M54">
+        <v>0</v>
+      </c>
+      <c r="N54">
+        <v>0</v>
+      </c>
+      <c r="O54">
+        <v>0</v>
+      </c>
+      <c r="P54">
+        <v>0</v>
+      </c>
+      <c r="Q54">
+        <v>0</v>
+      </c>
+      <c r="R54">
+        <v>0</v>
+      </c>
+      <c r="S54">
+        <v>0</v>
+      </c>
+      <c r="T54">
+        <v>0</v>
+      </c>
+      <c r="U54">
+        <v>0</v>
+      </c>
+      <c r="V54">
+        <v>0</v>
+      </c>
+      <c r="W54">
+        <v>0</v>
+      </c>
+      <c r="X54">
+        <v>0</v>
+      </c>
+      <c r="Y54">
+        <v>0</v>
+      </c>
+      <c r="Z54">
+        <v>0</v>
+      </c>
+      <c r="AA54">
+        <v>0</v>
+      </c>
+      <c r="AB54">
+        <v>0</v>
+      </c>
+      <c r="AC54">
+        <v>0</v>
+      </c>
+      <c r="AD54">
+        <v>0</v>
+      </c>
+      <c r="AE54">
+        <v>0</v>
+      </c>
+      <c r="AF54">
+        <v>0</v>
+      </c>
+      <c r="AG54">
+        <v>0</v>
+      </c>
+      <c r="AH54">
+        <v>0</v>
+      </c>
+      <c r="AI54">
+        <v>0</v>
+      </c>
+      <c r="AJ54">
+        <v>0</v>
+      </c>
+      <c r="AK54">
+        <v>0</v>
+      </c>
+      <c r="AL54">
+        <v>0</v>
+      </c>
+      <c r="AM54">
         <v>0</v>
       </c>
     </row>
@@ -6966,7 +7088,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T53"/>
+  <dimension ref="A1:T54"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -10252,6 +10374,68 @@
         <v>0</v>
       </c>
       <c r="T53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:20">
+      <c r="A54" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B54">
+        <v>0</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="E54">
+        <v>0</v>
+      </c>
+      <c r="F54">
+        <v>0</v>
+      </c>
+      <c r="G54">
+        <v>0</v>
+      </c>
+      <c r="H54">
+        <v>0</v>
+      </c>
+      <c r="I54">
+        <v>0</v>
+      </c>
+      <c r="J54">
+        <v>0</v>
+      </c>
+      <c r="K54">
+        <v>0</v>
+      </c>
+      <c r="L54">
+        <v>0</v>
+      </c>
+      <c r="M54">
+        <v>0</v>
+      </c>
+      <c r="N54">
+        <v>0</v>
+      </c>
+      <c r="O54">
+        <v>0</v>
+      </c>
+      <c r="P54">
+        <v>0</v>
+      </c>
+      <c r="Q54">
+        <v>0</v>
+      </c>
+      <c r="R54">
+        <v>0</v>
+      </c>
+      <c r="S54">
+        <v>0</v>
+      </c>
+      <c r="T54">
         <v>0</v>
       </c>
     </row>
@@ -10709,74 +10893,74 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>38</v>
+        <v>69</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>73.66</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>71.70999999999999</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>71.36</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>69.76000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>68</v>
+        <v>41</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>69.56</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>69.26000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>64.95999999999999</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>71</v>
+        <v>88</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>63.66</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>61.8</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -10784,63 +10968,63 @@
         <v>73</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>60.66</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>60.36</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>59.86</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>59.76</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
-        <v>77</v>
+        <v>38</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>59.56</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>58.51</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
-        <v>79</v>
+        <v>48</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>58.4</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>58.26</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -10848,279 +11032,279 @@
         <v>81</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>57.76</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="1" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
       <c r="B20">
-        <v>0</v>
+        <v>56.65</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="1" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B21">
-        <v>0</v>
+        <v>55.96</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="1" t="s">
-        <v>84</v>
+        <v>62</v>
       </c>
       <c r="B22">
-        <v>0</v>
+        <v>54.36</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="1" t="s">
-        <v>85</v>
+        <v>42</v>
       </c>
       <c r="B23">
-        <v>0</v>
+        <v>54.06</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="1" t="s">
-        <v>86</v>
+        <v>44</v>
       </c>
       <c r="B24">
-        <v>0</v>
+        <v>53.06</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="1" t="s">
-        <v>87</v>
+        <v>52</v>
       </c>
       <c r="B25">
-        <v>0</v>
+        <v>52.36</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="1" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="B26">
-        <v>0</v>
+        <v>51.05</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="1" t="s">
-        <v>65</v>
+        <v>84</v>
       </c>
       <c r="B27">
-        <v>0</v>
+        <v>50.76</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="1" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="B28">
-        <v>0</v>
+        <v>50.6</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="1" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
       <c r="B29">
-        <v>0</v>
+        <v>50.1</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="1" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="B30">
-        <v>0</v>
+        <v>49.16</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="1" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B31">
-        <v>0</v>
+        <v>48.46</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="1" t="s">
-        <v>41</v>
+        <v>72</v>
       </c>
       <c r="B32">
-        <v>0</v>
+        <v>48.06</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="1" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="B33">
-        <v>0</v>
+        <v>47.66</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B34">
-        <v>0</v>
+        <v>47.2</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="1" t="s">
-        <v>44</v>
+        <v>87</v>
       </c>
       <c r="B35">
-        <v>0</v>
+        <v>46.56</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="1" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="B36">
-        <v>0</v>
+        <v>45.86</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B37">
-        <v>0</v>
+        <v>45.46</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="1" t="s">
-        <v>47</v>
+        <v>80</v>
       </c>
       <c r="B38">
-        <v>0</v>
+        <v>45.3</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="1" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="B39">
-        <v>0</v>
+        <v>45.3</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="1" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B40">
-        <v>0</v>
+        <v>44.06</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="1" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="B41">
-        <v>0</v>
+        <v>43.1</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B42">
-        <v>0</v>
+        <v>41.6</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="1" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="B43">
-        <v>0</v>
+        <v>39.66</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="1" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="B44">
-        <v>0</v>
+        <v>39.66</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="1" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="B45">
-        <v>0</v>
+        <v>38.5</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="1" t="s">
-        <v>55</v>
+        <v>89</v>
       </c>
       <c r="B46">
-        <v>0</v>
+        <v>35.8</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="1" t="s">
-        <v>56</v>
+        <v>79</v>
       </c>
       <c r="B47">
-        <v>0</v>
+        <v>34.76</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="1" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="B48">
-        <v>0</v>
+        <v>34.36</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B49">
-        <v>0</v>
+        <v>30.32</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="1" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="B50">
-        <v>0</v>
+        <v>30.06</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="1" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="B51">
-        <v>0</v>
+        <v>26.51</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="1" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="B52">
-        <v>0</v>
+        <v>23.26</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" s="1" t="s">
-        <v>89</v>
+        <v>56</v>
       </c>
       <c r="B53">
-        <v>0</v>
+        <v>21.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>